<commit_message>
lecture: keyword_id -> question_keywords: foreign key로(lecture_id 대신 keyword_id)
</commit_message>
<xml_diff>
--- a/DB 프로젝트용 데이터 스키마.xlsx
+++ b/DB 프로젝트용 데이터 스키마.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/minji/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\남호\DBproj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{061F26DB-C861-7642-BC01-493D437CE70A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70136D55-89E3-436D-8E53-C44AF3B3AC33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16600" windowHeight="15840" xr2:uid="{E8AE0271-62BB-4733-BED4-D03C7E140794}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E8AE0271-62BB-4733-BED4-D03C7E140794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="89">
   <si>
     <t>TABLE_NAME</t>
   </si>
@@ -104,9 +104,6 @@
     <t>lecture_id</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>keyword</t>
   </si>
   <si>
@@ -362,6 +359,10 @@
   </si>
   <si>
     <t>문항 - 보기 테이블</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>keyword_id</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -369,7 +370,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -788,23 +789,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5410019B-4938-408A-B1D2-1440BE419DD7}">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="1" max="1" width="30.296875" customWidth="1"/>
     <col min="2" max="2" width="35.5" customWidth="1"/>
-    <col min="3" max="3" width="21.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.796875" customWidth="1"/>
     <col min="4" max="4" width="31.5" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" customWidth="1"/>
-    <col min="6" max="6" width="66.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.19921875" customWidth="1"/>
+    <col min="6" max="6" width="66.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,90 +822,90 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>65</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>66</v>
       </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -915,13 +916,13 @@
         <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -932,13 +933,13 @@
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -946,16 +947,16 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>69</v>
       </c>
-      <c r="E9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -966,472 +967,455 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
         <v>18</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
         <v>16</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>21</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
       </c>
       <c r="D18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
         <v>7</v>
       </c>
       <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
         <v>46</v>
       </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>47</v>
-      </c>
       <c r="E22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" t="s">
         <v>21</v>
       </c>
       <c r="D23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>80</v>
+      </c>
+      <c r="D25" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
         <v>34</v>
       </c>
-      <c r="C25" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
-      <c r="A27" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29" t="s">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>72</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" t="s">
+        <v>82</v>
+      </c>
+      <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
         <v>51</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C30" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>28</v>
-      </c>
-      <c r="B31" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>52</v>
       </c>
       <c r="E31" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D32" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
+        <v>76</v>
+      </c>
+      <c r="D33" t="s">
         <v>77</v>
       </c>
-      <c r="D33" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
         <v>21</v>
       </c>
       <c r="D34" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A36" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" t="s">
         <v>49</v>
       </c>
-      <c r="E34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" t="s">
-        <v>26</v>
-      </c>
-      <c r="D36" t="s">
-        <v>50</v>
-      </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="D37" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E37" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
+        <v>53</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A40" t="s">
+        <v>84</v>
+      </c>
+      <c r="B40" t="s">
+        <v>87</v>
+      </c>
+      <c r="C40" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A41" t="s">
+        <v>83</v>
+      </c>
+      <c r="B41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" t="s">
         <v>49</v>
       </c>
-      <c r="E38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" t="s">
-        <v>30</v>
-      </c>
-      <c r="B39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>85</v>
-      </c>
-      <c r="B41" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" t="s">
-        <v>82</v>
-      </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A42" t="s">
         <v>83</v>
       </c>
-      <c r="E41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="D42" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>84</v>
-      </c>
-      <c r="B43" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>75</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>